<commit_message>
add and edit datasets for age and gender
</commit_message>
<xml_diff>
--- a/datasets/canada-lendingrates-2000to2020.xlsx
+++ b/datasets/canada-lendingrates-2000to2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MMS-012\Documents\GitHub\TorontoHousingMarket\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04E9623-9A42-4E89-98D4-026C7B50597D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9830F43E-137F-4D9D-904F-F1676A2876C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{9C3043CE-986E-491D-912B-107530680938}"/>
   </bookViews>
@@ -36,10 +36,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Percent</t>
+    <t>Month</t>
   </si>
   <si>
-    <t>Month</t>
+    <t>Lending Rate</t>
   </si>
 </sst>
 </file>
@@ -93,6 +93,2361 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lending Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$250</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="249"/>
+                <c:pt idx="0">
+                  <c:v>36526</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36557</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36586</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>36617</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36647</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>36678</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36708</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36739</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>36770</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>36831</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36861</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>36892</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36923</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36951</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>36982</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>37012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>37043</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37073</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>37104</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>37135</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>37165</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>37196</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>37226</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>37257</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>37288</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>37316</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37347</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37377</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37408</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>37438</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>37469</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>37500</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37530</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>37561</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37591</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37622</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37653</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>37681</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>37712</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>37742</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>37773</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>37803</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>37834</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>37865</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>37895</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>37926</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>37956</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>37987</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>38018</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>38047</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>38078</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>38108</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>38139</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>38169</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>38200</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>38231</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>38261</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>38292</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>38322</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>38353</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>38384</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>38412</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>38443</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>38473</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>38504</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>38534</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>38565</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>38596</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>38626</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>38657</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>38687</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>38718</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>38749</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>38777</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>38808</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>38838</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>38869</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>38899</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>38930</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>38961</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>38991</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>39022</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>39052</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>39083</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>39114</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>39142</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>39173</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>39203</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>39234</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>39264</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>39295</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>39326</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>39356</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>39387</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>39417</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>39448</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>39479</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>39508</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>39539</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>39569</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>39600</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>39630</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>39661</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>39692</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>39722</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>39753</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>39783</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>39814</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>39845</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>39873</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>39904</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>39934</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>39965</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>39995</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>40026</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>40057</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>40087</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>40118</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>40148</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>40179</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>40210</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>40238</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>40269</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>40299</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>40330</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>40360</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>40391</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>40422</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>40452</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>40483</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>40513</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>40544</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>40575</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>40603</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>40634</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>40664</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>40695</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>40725</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>40756</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>40787</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>40817</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>40848</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>40878</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>40909</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>40940</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>40969</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>41000</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>41030</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>41061</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>41091</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>41122</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>41153</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>41183</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>41214</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>41244</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>41275</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>41306</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>41334</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>41365</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>41395</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>41426</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>41456</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>41487</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>41518</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>41548</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>41579</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>41609</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>41640</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>41671</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>41699</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>41730</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>41760</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>41791</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>41821</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>41852</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>41883</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>41913</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>41944</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>41974</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>42005</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>42036</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>42064</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>42095</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>42125</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>42156</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>42186</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>42217</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>42248</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>42278</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>42309</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>42339</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>42370</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>42401</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>42430</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>42461</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>42491</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>42522</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>42552</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>42583</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>42614</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>42644</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>42705</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>42736</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>42767</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>42795</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>42826</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>42856</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>42887</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>42917</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>42948</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>42979</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>43009</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>43040</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>43070</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>43252</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>43282</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>43313</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>43344</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>43374</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>43405</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>43435</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>43466</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>43525</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>43556</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>43617</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>43647</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>43678</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>43709</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>43739</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>43770</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>43800</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>43831</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>43862</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>43891</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>43922</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>43952</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>43983</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>44013</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>44044</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>44075</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$250</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="249"/>
+                <c:pt idx="0">
+                  <c:v>8.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.43</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.34</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.08</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.08</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.0399999999999991</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.81</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.58</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.52</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.22</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.38</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.47</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.46</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.39</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.03</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.74</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.51</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.64</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6.62</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.59</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.98</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.9</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.61</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6.49</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>6.47</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>6.39</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>6.26</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.29</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>6.33</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>6.44</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.62</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.71</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.87</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.97</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.83</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6.02</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.78</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.51</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5.31</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.82</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.06</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.97</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.94</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.95</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.87</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.69</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.59</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.67</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.55</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.31</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.26</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>5.32</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>5.39</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>5.56</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.65</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>5.78</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.88</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>6.05</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>6.12</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>6.26</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6.24</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>6.13</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.01</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5.99</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5.89</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5.91</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.91</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>5.92</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>6.01</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>6.51</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6.62</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>6.61</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6.69</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6.73</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>6.81</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>6.72</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>6.21</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>6.37</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>6.16</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>6.46</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>6.51</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>6.17</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>5.78</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>5.28</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>5.14</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>4.79</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>5.14</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>5.13</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>4.97</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>5.0599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>4.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>5.15</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>5.18</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>5.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>4.82</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>4.45</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>4.55</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>4.68</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>4.87</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>4.57</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>4.3600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4.3099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>4.2300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>4.21</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>4.3600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>4.2300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>4.2300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>4.17</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>4.1500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>4.1500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>4.1399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>4.1100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>4.1399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>4.33</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>4.32</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>4.16</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>4.01</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>4.0199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>3.98</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>3.96</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>3.84</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>3.76</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>3.74</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>3.71</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>3.76</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>3.73</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>3.67</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>3.67</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>3.68</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>3.67</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>3.68</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>3.74</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>3.73</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>3.62</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>3.59</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>3.82</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>3.89</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>3.98</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>4.04</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>4.07</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>4.1399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>4.26</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>4.2699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4.2699999999999996</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>4.32</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>4.42</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>4.4800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>4.38</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>4.59</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>4.59</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>4.4400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>4.33</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>4.2300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>4.1399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>4.07</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>4.09</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>4.09</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>4.08</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>3.95</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>3.86</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>3.77</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>3.64</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>3.57</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>3.51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-423F-4289-8964-F631FF3BEE16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="433362703"/>
+        <c:axId val="657395599"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="433362703"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="657395599"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="657395599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433362703"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>536575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>231775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3849B2AB-33E8-427B-BFD1-EE9B3561E2AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,18 +2749,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86063B2A-C044-4ADA-8AD5-1C015EC46F18}">
   <dimension ref="A1:IR250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:252" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:252" x14ac:dyDescent="0.35">
@@ -2648,5 +5003,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>